<commit_message>
Result files and graphs
</commit_message>
<xml_diff>
--- a/TetrisExperiments.xlsx
+++ b/TetrisExperiments.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>Weights</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Raph</t>
   </si>
   <si>
-    <t>Oscar</t>
-  </si>
-  <si>
     <t>Ravg - Havg - (200 - Aavg)</t>
   </si>
   <si>
@@ -86,55 +83,35 @@
     <t>fitness function from the paper</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">30 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Error, d</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>id 15 instead</t>
-    </r>
-  </si>
-  <si>
-    <t>Oscar PSO_30_500_04-14-17.48.02</t>
-  </si>
-  <si>
-    <t>Oscar PSO_150_100_04-14-17.48.02</t>
-  </si>
-  <si>
     <t>Oscar (One look ahead) PSO_30_150_04-14-23.56.01</t>
   </si>
   <si>
     <t>Ash (One look ahead) PSO_30_150_04-15-00.13.02</t>
   </si>
   <si>
-    <t>Ash Aish_PSO_30_500_04-14-18.47.01</t>
-  </si>
-  <si>
-    <t>Ash WRONG_PSO_15_100_04-14-18.47.01</t>
-  </si>
-  <si>
-    <t>Ash PSO_30_500_04-15-01.36.02</t>
+    <t>PSO_30_500_04-14-17.48.02_Oscar</t>
+  </si>
+  <si>
+    <t>PSO_150_100_04-14-17.48.02_Oscar</t>
+  </si>
+  <si>
+    <t>PSO_30_100_04-15-01.46.02_Oscar</t>
+  </si>
+  <si>
+    <t>PSO_30_500_04-15-01.36.02_Aish</t>
+  </si>
+  <si>
+    <t>PSO_30_500_04-14-18.47.01_Aish</t>
+  </si>
+  <si>
+    <t>Oscar PSO_1st_attempt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,18 +139,6 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri (Body)"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -488,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -526,7 +491,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -668,13 +633,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
       </c>
       <c r="D10">
         <v>30</v>
@@ -685,13 +650,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>30</v>
@@ -702,16 +667,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <v>30</v>
       </c>
       <c r="E12">
         <v>100</v>
@@ -725,7 +690,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13">
         <v>30</v>
@@ -734,26 +699,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14">
-        <v>30</v>
-      </c>
-      <c r="E14">
-        <v>100</v>
-      </c>
-    </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -770,13 +718,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16">
         <v>30</v>

</xml_diff>